<commit_message>
update export logic with removed date column
</commit_message>
<xml_diff>
--- a/src/assets/templates/JUSTIFI_project_template.xlsx
+++ b/src/assets/templates/JUSTIFI_project_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/Documents/NEB-Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/dev/AMO-Tools-Desktop/src/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9C3A294-FF0A-3247-8BC9-78D3A9149CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B90CFD0-0640-A542-9E9E-7353C6B6B30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" activeTab="5" xr2:uid="{A9E208C3-F2B3-F746-8822-8A28C5BC2449}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" activeTab="4" xr2:uid="{A9E208C3-F2B3-F746-8822-8A28C5BC2449}"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="145">
   <si>
     <t>Facility Data</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Assessment Type</t>
-  </si>
-  <si>
-    <t>Assessment Date</t>
   </si>
   <si>
     <t>Cost/Savings Data level</t>
@@ -722,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -751,7 +748,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1542,26 +1538,26 @@
       <c r="F1" s="18"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2056,41 +2052,41 @@
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
     </row>
-    <row r="2" spans="1:12" s="27" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:12" s="26" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="25" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3124,14 +3120,14 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
@@ -3643,960 +3639,935 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A06F1A4-B22D-6C47-94C6-89CA9E21F2FE}">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="18.1640625" customWidth="1"/>
-    <col min="24" max="24" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.6640625" hidden="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" style="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.6640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="17" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="17" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18"/>
-    </row>
-    <row r="2" spans="1:26" s="29" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:25" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="P2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="T2" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="29" t="s">
+      <c r="U2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="V2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="X2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="Y2" s="29" t="s">
+      <c r="Y2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="Z2" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="14"/>
       <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J3" s="12"/>
       <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S3" s="12"/>
       <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="14" t="s">
+      <c r="U3" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V3" s="12"/>
       <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="14" t="s">
+      <c r="X3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="12"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y3" s="12"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="14"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M4" s="12"/>
       <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" s="12"/>
       <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="14" t="s">
+      <c r="U4" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V4" s="12"/>
       <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="14" t="s">
+      <c r="X4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y4" s="12"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="14"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M5" s="12"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="12"/>
       <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="14" t="s">
+      <c r="U5" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V5" s="12"/>
       <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="14" t="s">
+      <c r="X5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="12"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y5" s="12"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J6" s="12"/>
       <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M6" s="12"/>
       <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" s="12"/>
       <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="14" t="s">
+      <c r="U6" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V6" s="12"/>
       <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="14" t="s">
+      <c r="X6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z6" s="12"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y6" s="12"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M7" s="12"/>
       <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" s="12"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="14" t="s">
+      <c r="U7" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V7" s="12"/>
       <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="14" t="s">
+      <c r="X7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z7" s="12"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y7" s="12"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="14"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J8" s="12"/>
       <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O8" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R8" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" s="12"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="14" t="s">
+      <c r="U8" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V8" s="12"/>
       <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="14" t="s">
+      <c r="X8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="12"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y8" s="12"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="14"/>
       <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J9" s="12"/>
       <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M9" s="12"/>
       <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" s="12"/>
       <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="14" t="s">
+      <c r="U9" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V9" s="12"/>
       <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="14" t="s">
+      <c r="X9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z9" s="12"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y9" s="12"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="14"/>
       <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J10" s="12"/>
       <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="14" t="s">
+      <c r="L10" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M10" s="12"/>
       <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S10" s="12"/>
       <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="14" t="s">
+      <c r="U10" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V10" s="12"/>
       <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="14" t="s">
+      <c r="X10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z10" s="12"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y10" s="12"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="14"/>
       <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M11" s="12"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" s="12"/>
       <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="14" t="s">
+      <c r="U11" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V11" s="12"/>
       <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="14" t="s">
+      <c r="X11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z11" s="12"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y11" s="12"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="14"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="14" t="s">
+      <c r="L12" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M12" s="12"/>
       <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" s="12"/>
       <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="14" t="s">
+      <c r="U12" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V12" s="12"/>
       <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="14" t="s">
+      <c r="X12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z12" s="12"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y12" s="12"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="14"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="14" t="s">
+      <c r="I13" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="14" t="s">
+      <c r="L13" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M13" s="12"/>
       <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S13" s="12"/>
       <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="14" t="s">
+      <c r="U13" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V13" s="12"/>
       <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="14" t="s">
+      <c r="X13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z13" s="12"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y13" s="12"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="14"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O14" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R14" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S14" s="12"/>
       <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="14" t="s">
+      <c r="U14" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V14" s="12"/>
       <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="14" t="s">
+      <c r="X14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z14" s="12"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y14" s="12"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="14"/>
       <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J15" s="12"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="14" t="s">
+      <c r="L15" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M15" s="12"/>
       <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R15" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S15" s="12"/>
       <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="14" t="s">
+      <c r="U15" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V15" s="12"/>
       <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="14" t="s">
+      <c r="X15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z15" s="12"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="14"/>
       <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14" t="s">
+      <c r="F16" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="14" t="s">
+      <c r="I16" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J16" s="12"/>
       <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M16" s="12"/>
       <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S16" s="12"/>
       <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="14" t="s">
+      <c r="U16" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V16" s="12"/>
       <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="14" t="s">
+      <c r="X16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z16" s="12"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y16" s="12"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="14"/>
       <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J17" s="12"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="14" t="s">
+      <c r="L17" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M17" s="12"/>
       <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S17" s="12"/>
       <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="14" t="s">
+      <c r="U17" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V17" s="12"/>
       <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="14" t="s">
+      <c r="X17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z17" s="12"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y17" s="12"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="14"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="14" t="s">
+      <c r="F18" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="14" t="s">
+      <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J18" s="12"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="14" t="s">
+      <c r="L18" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M18" s="12"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O18" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R18" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S18" s="12"/>
       <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="14" t="s">
+      <c r="U18" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V18" s="12"/>
       <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="14" t="s">
+      <c r="X18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z18" s="12"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y18" s="12"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="14"/>
       <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="14" t="s">
+      <c r="I19" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="14" t="s">
+      <c r="L19" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M19" s="12"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S19" s="12"/>
       <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="14" t="s">
+      <c r="U19" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V19" s="12"/>
       <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="14" t="s">
+      <c r="X19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z19" s="12"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y19" s="12"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="14"/>
       <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="14" t="s">
+      <c r="F20" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="14" t="s">
+      <c r="I20" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J20" s="12"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="14" t="s">
+      <c r="L20" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M20" s="12"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S20" s="12"/>
       <c r="T20" s="12"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="14" t="s">
+      <c r="U20" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V20" s="12"/>
       <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="14" t="s">
+      <c r="X20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z20" s="12"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Y20" s="12"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="14"/>
       <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="14" t="s">
+      <c r="F21" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="14" t="s">
+      <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="J21" s="12"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="14" t="s">
+      <c r="L21" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="M21" s="12"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="O21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="14" t="s">
-        <v>75</v>
-      </c>
+      <c r="R21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" s="12"/>
       <c r="T21" s="12"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="14" t="s">
+      <c r="U21" s="14" t="s">
         <v>25</v>
       </c>
+      <c r="V21" s="12"/>
       <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="14" t="s">
+      <c r="X21" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Z21" s="12"/>
-    </row>
-    <row r="22" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="Y21" s="12"/>
+    </row>
+    <row r="22" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A3:Z21">
+  <conditionalFormatting sqref="A3:Y21">
     <cfRule type="expression" dxfId="7" priority="5">
       <formula>$A2 = ""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E21 H3:H21 K3:K21 N3:N21 Q3:Q21 T3:T21 W3:W21 Z3:Z21">
+  <conditionalFormatting sqref="D3:D21 G3:G21 J3:J21 M3:M21 P3:P21 S3:S21 V3:V21 Y3:Y21">
     <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$D3="Individual"</formula>
+      <formula>$C3="Individual"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:N21">
+  <conditionalFormatting sqref="H3:M21">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>OR($B3 = "Pump", $B3 = "Fan",$B3 = "Motor",$B3 = "Lighting", $B3 = "Compressed Air")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:T21">
+  <conditionalFormatting sqref="N3:S21">
     <cfRule type="expression" dxfId="4" priority="3">
       <formula>OR($B3 = "Fan",$B3 = "Motor",$B3 = "Lighting", $B3 = "Compressed Air",  $B3 = "Mobile")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:W21">
+  <conditionalFormatting sqref="T3:V21">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>OR($B3 = "Pump", $B3 = "Fan",$B3 = "Motor",$B3 = "Lighting", $B3 = "Process Cooling",  $B3 = "Mobile",  $B3 = "HVAC",$B3 = "Process Heating", $B3 = "Steam" )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:Z21">
+  <conditionalFormatting sqref="W3:Y21">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>OR($B3 = "Pump", $B3 = "Fan",$B3 = "Motor",$B3 = "Lighting", $B3 = "Process Cooling",  $B3 = "Mobile",  $B3 = "HVAC",$B3 = "Compressed Air" )</formula>
     </cfRule>
@@ -4605,19 +4576,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B21" xr:uid="{AC30697D-BCFD-45D9-B5BF-FCA65920BF2C}">
       <formula1>Names_Assessments</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D21" xr:uid="{A3F9B353-4D25-4892-A908-553DDF73FC2E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C21" xr:uid="{A3F9B353-4D25-4892-A908-553DDF73FC2E}">
       <formula1>"Individual, Assessment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J21 G3:G21 M3:M21" xr:uid="{33BDF14F-6C28-418A-9B91-5827556CE11C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I21 F3:F21 L3:L21" xr:uid="{33BDF14F-6C28-418A-9B91-5827556CE11C}">
       <formula1>Units_Energy</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S21 P3:P21" xr:uid="{5CFA88FA-87FD-4E4C-BA74-9E96632A03F9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R21 O3:O21" xr:uid="{5CFA88FA-87FD-4E4C-BA74-9E96632A03F9}">
       <formula1>Units_Water</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y21" xr:uid="{719235EB-1DD6-471D-8709-1CD65CA66A3F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X21" xr:uid="{719235EB-1DD6-471D-8709-1CD65CA66A3F}">
       <formula1>Units_Steam</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V21" xr:uid="{96B900EE-4BF7-48C3-975C-A5EEDFE3E7F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U21" xr:uid="{96B900EE-4BF7-48C3-975C-A5EEDFE3E7F0}">
       <formula1>Units_Compressed_Air</formula1>
     </dataValidation>
   </dataValidations>
@@ -4629,7 +4600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D738118F-2EBE-D044-8200-FB4EC4565940}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -4665,7 +4636,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -4677,33 +4648,33 @@
       <c r="I1" s="18"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="2" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
@@ -5284,7 +5255,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="12" t="e">
-        <f t="shared" ref="B35:B66" si="2">VLOOKUP(_xlfn.XMATCH(A35,Lookup_AssessmentList),Lookup_Assessment,3)</f>
+        <f t="shared" ref="B35:B51" si="2">VLOOKUP(_xlfn.XMATCH(A35,Lookup_AssessmentList),Lookup_Assessment,3)</f>
         <v>#N/A</v>
       </c>
       <c r="C35" s="12" t="e">
@@ -5626,31 +5597,31 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>85</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>86</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>87</v>
-      </c>
-      <c r="K2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -5658,25 +5629,25 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
         <v>91</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>91</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" t="s">
-        <v>92</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
@@ -5684,28 +5655,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>95</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>96</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>97</v>
       </c>
-      <c r="H4" t="s">
-        <v>98</v>
-      </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K4" t="s">
         <v>16</v>
@@ -5713,42 +5684,42 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>99</v>
       </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>101</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>102</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>103</v>
-      </c>
-      <c r="I5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>108</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -5759,19 +5730,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" t="s">
         <v>110</v>
-      </c>
-      <c r="E7" t="s">
-        <v>111</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
@@ -5782,62 +5753,62 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
         <v>112</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
         <v>114</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>115</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>116</v>
-      </c>
-      <c r="I8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
         <v>118</v>
       </c>
-      <c r="C9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>119</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>120</v>
       </c>
-      <c r="H9" t="s">
-        <v>121</v>
-      </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
         <v>122</v>
       </c>
-      <c r="C10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>123</v>
       </c>
-      <c r="H10" t="s">
-        <v>124</v>
-      </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -5845,24 +5816,24 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
         <v>125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" t="s">
         <v>127</v>
-      </c>
-      <c r="C12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" t="s">
-        <v>128</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
@@ -5870,23 +5841,23 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -5896,48 +5867,48 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" t="s">
         <v>130</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>131</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>132</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>133</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>134</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>135</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>136</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>137</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>138</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>139</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>140</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>141</v>
-      </c>
-      <c r="M22" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -6094,13 +6065,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
         <v>143</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>144</v>
-      </c>
-      <c r="C30" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -6112,7 +6083,7 @@
         <v>Assessments</v>
       </c>
       <c r="C31" s="21">
-        <f>Assessments!D3</f>
+        <f>Assessments!C3</f>
         <v>0</v>
       </c>
       <c r="D31" t="str">
@@ -6129,7 +6100,7 @@
         <v>Assessments</v>
       </c>
       <c r="C32" s="21">
-        <f>Assessments!D4</f>
+        <f>Assessments!C4</f>
         <v>0</v>
       </c>
       <c r="D32" t="str">
@@ -6146,7 +6117,7 @@
         <v>Assessments</v>
       </c>
       <c r="C33" s="21">
-        <f>Assessments!D5</f>
+        <f>Assessments!C5</f>
         <v>0</v>
       </c>
       <c r="D33" t="str">
@@ -6163,7 +6134,7 @@
         <v>Assessments</v>
       </c>
       <c r="C34" s="21">
-        <f>Assessments!D6</f>
+        <f>Assessments!C6</f>
         <v>0</v>
       </c>
       <c r="D34" t="str">
@@ -6180,7 +6151,7 @@
         <v>Assessments</v>
       </c>
       <c r="C35" s="21">
-        <f>Assessments!D7</f>
+        <f>Assessments!C7</f>
         <v>0</v>
       </c>
       <c r="D35" t="str">
@@ -6197,7 +6168,7 @@
         <v>Assessments</v>
       </c>
       <c r="C36" s="21">
-        <f>Assessments!D8</f>
+        <f>Assessments!C8</f>
         <v>0</v>
       </c>
       <c r="D36" t="str">
@@ -6214,7 +6185,7 @@
         <v>Assessments</v>
       </c>
       <c r="C37" s="21">
-        <f>Assessments!D9</f>
+        <f>Assessments!C9</f>
         <v>0</v>
       </c>
       <c r="D37" t="str">
@@ -6231,7 +6202,7 @@
         <v>Assessments</v>
       </c>
       <c r="C38" s="21">
-        <f>Assessments!D10</f>
+        <f>Assessments!C10</f>
         <v>0</v>
       </c>
       <c r="D38" t="str">
@@ -6248,7 +6219,7 @@
         <v>Assessments</v>
       </c>
       <c r="C39" s="21">
-        <f>Assessments!D11</f>
+        <f>Assessments!C11</f>
         <v>0</v>
       </c>
       <c r="D39" t="str">
@@ -6265,7 +6236,7 @@
         <v>Assessments</v>
       </c>
       <c r="C40" s="21">
-        <f>Assessments!D12</f>
+        <f>Assessments!C12</f>
         <v>0</v>
       </c>
       <c r="D40" t="str">
@@ -6282,7 +6253,7 @@
         <v>Assessments</v>
       </c>
       <c r="C41" s="21">
-        <f>Assessments!D13</f>
+        <f>Assessments!C13</f>
         <v>0</v>
       </c>
       <c r="D41" t="str">
@@ -6299,7 +6270,7 @@
         <v>Assessments</v>
       </c>
       <c r="C42" s="21">
-        <f>Assessments!D14</f>
+        <f>Assessments!C14</f>
         <v>0</v>
       </c>
       <c r="D42" t="str">
@@ -6316,7 +6287,7 @@
         <v>Assessments</v>
       </c>
       <c r="C43" s="21">
-        <f>Assessments!D15</f>
+        <f>Assessments!C15</f>
         <v>0</v>
       </c>
       <c r="D43" t="str">
@@ -6333,7 +6304,7 @@
         <v>Assessments</v>
       </c>
       <c r="C44" s="21">
-        <f>Assessments!D16</f>
+        <f>Assessments!C16</f>
         <v>0</v>
       </c>
       <c r="D44" t="str">
@@ -6350,7 +6321,7 @@
         <v>Assessments</v>
       </c>
       <c r="C45" s="21">
-        <f>Assessments!D17</f>
+        <f>Assessments!C17</f>
         <v>0</v>
       </c>
       <c r="D45" t="str">
@@ -6367,7 +6338,7 @@
         <v>Assessments</v>
       </c>
       <c r="C46" s="21">
-        <f>Assessments!D18</f>
+        <f>Assessments!C18</f>
         <v>0</v>
       </c>
       <c r="D46" t="str">
@@ -6384,7 +6355,7 @@
         <v>Assessments</v>
       </c>
       <c r="C47" s="21">
-        <f>Assessments!D19</f>
+        <f>Assessments!C19</f>
         <v>0</v>
       </c>
       <c r="D47" t="str">
@@ -6401,7 +6372,7 @@
         <v>Assessments</v>
       </c>
       <c r="C48" s="21">
-        <f>Assessments!D20</f>
+        <f>Assessments!C20</f>
         <v>0</v>
       </c>
       <c r="D48" t="str">
@@ -6418,7 +6389,7 @@
         <v>Assessments</v>
       </c>
       <c r="C49" s="21">
-        <f>Assessments!D21</f>
+        <f>Assessments!C21</f>
         <v>0</v>
       </c>
       <c r="D49" t="str">
@@ -6435,7 +6406,7 @@
         <v>Assessments</v>
       </c>
       <c r="C50" s="21">
-        <f>Assessments!D22</f>
+        <f>Assessments!C22</f>
         <v>0</v>
       </c>
       <c r="D50" t="str">
@@ -6452,7 +6423,7 @@
         <v>Assessments</v>
       </c>
       <c r="C51" s="21">
-        <f>Assessments!D23</f>
+        <f>Assessments!C23</f>
         <v>0</v>
       </c>
       <c r="D51" t="str">
@@ -6469,7 +6440,7 @@
         <v>Assessments</v>
       </c>
       <c r="C52" s="21">
-        <f>Assessments!D24</f>
+        <f>Assessments!C24</f>
         <v>0</v>
       </c>
       <c r="D52" t="str">
@@ -6486,7 +6457,7 @@
         <v>Assessments</v>
       </c>
       <c r="C53" s="21">
-        <f>Assessments!D25</f>
+        <f>Assessments!C25</f>
         <v>0</v>
       </c>
       <c r="D53" t="str">
@@ -6503,7 +6474,7 @@
         <v>Assessments</v>
       </c>
       <c r="C54" s="21">
-        <f>Assessments!D26</f>
+        <f>Assessments!C26</f>
         <v>0</v>
       </c>
       <c r="D54" t="str">
@@ -6520,7 +6491,7 @@
         <v>Assessments</v>
       </c>
       <c r="C55" s="21">
-        <f>Assessments!D27</f>
+        <f>Assessments!C27</f>
         <v>0</v>
       </c>
       <c r="D55" t="str">
@@ -6537,7 +6508,7 @@
         <v>Assessments</v>
       </c>
       <c r="C56" s="21">
-        <f>Assessments!D28</f>
+        <f>Assessments!C28</f>
         <v>0</v>
       </c>
       <c r="D56" t="str">
@@ -6554,7 +6525,7 @@
         <v>Assessments</v>
       </c>
       <c r="C57" s="21">
-        <f>Assessments!D29</f>
+        <f>Assessments!C29</f>
         <v>0</v>
       </c>
       <c r="D57" t="str">
@@ -6571,7 +6542,7 @@
         <v>Assessments</v>
       </c>
       <c r="C58" s="21">
-        <f>Assessments!D30</f>
+        <f>Assessments!C30</f>
         <v>0</v>
       </c>
       <c r="D58" t="str">
@@ -6588,7 +6559,7 @@
         <v>Assessments</v>
       </c>
       <c r="C59" s="21">
-        <f>Assessments!D31</f>
+        <f>Assessments!C31</f>
         <v>0</v>
       </c>
       <c r="D59" t="str">
@@ -6605,7 +6576,7 @@
         <v>Assessments</v>
       </c>
       <c r="C60" s="21">
-        <f>Assessments!D32</f>
+        <f>Assessments!C32</f>
         <v>0</v>
       </c>
       <c r="D60" t="str">
@@ -6622,7 +6593,7 @@
         <v>Assessments</v>
       </c>
       <c r="C61" s="21">
-        <f>Assessments!D33</f>
+        <f>Assessments!C33</f>
         <v>0</v>
       </c>
       <c r="D61" t="str">
@@ -6639,7 +6610,7 @@
         <v>Assessments</v>
       </c>
       <c r="C62" s="21">
-        <f>Assessments!D34</f>
+        <f>Assessments!C34</f>
         <v>0</v>
       </c>
       <c r="D62" t="str">
@@ -6656,7 +6627,7 @@
         <v>Assessments</v>
       </c>
       <c r="C63" s="21">
-        <f>Assessments!D35</f>
+        <f>Assessments!C35</f>
         <v>0</v>
       </c>
       <c r="D63" t="str">
@@ -6673,7 +6644,7 @@
         <v>Assessments</v>
       </c>
       <c r="C64" s="21">
-        <f>Assessments!D36</f>
+        <f>Assessments!C36</f>
         <v>0</v>
       </c>
       <c r="D64" t="str">
@@ -6690,7 +6661,7 @@
         <v>Assessments</v>
       </c>
       <c r="C65" s="21">
-        <f>Assessments!D37</f>
+        <f>Assessments!C37</f>
         <v>0</v>
       </c>
       <c r="D65" t="str">
@@ -6707,7 +6678,7 @@
         <v>Assessments</v>
       </c>
       <c r="C66" s="21">
-        <f>Assessments!D38</f>
+        <f>Assessments!C38</f>
         <v>0</v>
       </c>
       <c r="D66" t="str">
@@ -6724,7 +6695,7 @@
         <v>Assessments</v>
       </c>
       <c r="C67" s="21">
-        <f>Assessments!D39</f>
+        <f>Assessments!C39</f>
         <v>0</v>
       </c>
       <c r="D67" t="str">
@@ -6741,7 +6712,7 @@
         <v>Assessments</v>
       </c>
       <c r="C68" s="21">
-        <f>Assessments!D40</f>
+        <f>Assessments!C40</f>
         <v>0</v>
       </c>
       <c r="D68" t="str">
@@ -6758,7 +6729,7 @@
         <v>Assessments</v>
       </c>
       <c r="C69" s="21">
-        <f>Assessments!D41</f>
+        <f>Assessments!C41</f>
         <v>0</v>
       </c>
       <c r="D69" t="str">
@@ -6775,7 +6746,7 @@
         <v>Assessments</v>
       </c>
       <c r="C70" s="21">
-        <f>Assessments!D42</f>
+        <f>Assessments!C42</f>
         <v>0</v>
       </c>
       <c r="D70" t="str">
@@ -6792,7 +6763,7 @@
         <v>Assessments</v>
       </c>
       <c r="C71" s="21">
-        <f>Assessments!D43</f>
+        <f>Assessments!C43</f>
         <v>0</v>
       </c>
       <c r="D71" t="str">
@@ -6809,7 +6780,7 @@
         <v>Assessments</v>
       </c>
       <c r="C72" s="21">
-        <f>Assessments!D44</f>
+        <f>Assessments!C44</f>
         <v>0</v>
       </c>
       <c r="D72" t="str">
@@ -6826,7 +6797,7 @@
         <v>Assessments</v>
       </c>
       <c r="C73" s="21">
-        <f>Assessments!D45</f>
+        <f>Assessments!C45</f>
         <v>0</v>
       </c>
       <c r="D73" t="str">
@@ -6843,7 +6814,7 @@
         <v>Assessments</v>
       </c>
       <c r="C74" s="21">
-        <f>Assessments!D46</f>
+        <f>Assessments!C46</f>
         <v>0</v>
       </c>
       <c r="D74" t="str">
@@ -6860,7 +6831,7 @@
         <v>Assessments</v>
       </c>
       <c r="C75" s="21">
-        <f>Assessments!D47</f>
+        <f>Assessments!C47</f>
         <v>0</v>
       </c>
       <c r="D75" t="str">
@@ -6877,7 +6848,7 @@
         <v>Assessments</v>
       </c>
       <c r="C76" s="21">
-        <f>Assessments!D48</f>
+        <f>Assessments!C48</f>
         <v>0</v>
       </c>
       <c r="D76" t="str">
@@ -6894,7 +6865,7 @@
         <v>Assessments</v>
       </c>
       <c r="C77" s="21">
-        <f>Assessments!D49</f>
+        <f>Assessments!C49</f>
         <v>0</v>
       </c>
       <c r="D77" t="str">
@@ -6911,7 +6882,7 @@
         <v>Assessments</v>
       </c>
       <c r="C78" s="21">
-        <f>Assessments!D50</f>
+        <f>Assessments!C50</f>
         <v>0</v>
       </c>
       <c r="D78" t="str">
@@ -6928,7 +6899,7 @@
         <v>Assessments</v>
       </c>
       <c r="C79" s="21">
-        <f>Assessments!D51</f>
+        <f>Assessments!C51</f>
         <v>0</v>
       </c>
       <c r="D79" t="str">
@@ -6945,7 +6916,7 @@
         <v>Assessments</v>
       </c>
       <c r="C80" s="21">
-        <f>Assessments!D52</f>
+        <f>Assessments!C52</f>
         <v>0</v>
       </c>
       <c r="D80" t="str">

</xml_diff>